<commit_message>
test on test branch
</commit_message>
<xml_diff>
--- a/Bug-Reports.xlsx
+++ b/Bug-Reports.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Татьяна\Bug-reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B39AEE-405E-4FE2-8A55-13224D6F091A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9C9E95-5C65-43D2-A5DF-460AA79184FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2544" yWindow="2544" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>ID</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>На странице "Введите код из письма" есть кнопка Назад для возврата на предыдущую страницу с целью поменять адрес почты</t>
+  </si>
+  <si>
+    <t>A7</t>
   </si>
 </sst>
 </file>
@@ -692,7 +695,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>